<commit_message>
adding mirai binaries download ACEs to MTD
</commit_message>
<xml_diff>
--- a/experiment/data/mirai_mtd.xlsx
+++ b/experiment/data/mirai_mtd.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="66">
   <si>
     <t xml:space="preserve">Group</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t xml:space="preserve">local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bin_download_from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bin_download_to</t>
   </si>
 </sst>
 </file>
@@ -223,7 +229,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -258,12 +264,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -308,7 +308,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -326,14 +326,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2142,8 +2134,8 @@
   </sheetPr>
   <dimension ref="A1:R1006"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P18" activeCellId="0" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2158,7 +2150,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.56"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="47.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="47.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="17.83"/>
@@ -2244,7 +2236,7 @@
       </c>
       <c r="P2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H2,"'}, ")</f>
-        <v>'tp_dst':'443'}, </v>
+        <v>'tp_dst':'443'},</v>
       </c>
       <c r="R2" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("echo '$USR|",C2," ",E2," $TEMPO dport=",H2,"' |  $NC; sleep $((2*$TEMPO));")</f>
@@ -2264,7 +2256,7 @@
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>52</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -2273,7 +2265,7 @@
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="6" t="n">
+      <c r="H3" s="1" t="n">
         <v>27015</v>
       </c>
       <c r="J3" s="1" t="str">
@@ -2302,7 +2294,7 @@
       </c>
       <c r="P3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H3,"'}, ")</f>
-        <v>'tp_dst':'27015'}, </v>
+        <v>'tp_dst':'27015'},</v>
       </c>
       <c r="R3" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("echo '$USR|",C3," ",E3," $TEMPO dport=",H3,"' |  $NC; sleep $((2*$TEMPO));")</f>
@@ -2360,7 +2352,7 @@
       </c>
       <c r="P4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H4,"'}, ")</f>
-        <v>'tp_dst':'123'}, </v>
+        <v>'tp_dst':'123'},</v>
       </c>
       <c r="R4" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("echo '$USR|",C4," ",E4," $TEMPO dport=",H4,"' |  $NC; sleep $((2*$TEMPO));")</f>
@@ -2418,7 +2410,7 @@
       </c>
       <c r="P5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H5,"'}, ")</f>
-        <v>'tp_dst':'80'}, </v>
+        <v>'tp_dst':'80'},</v>
       </c>
       <c r="R5" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("echo '$USR|",C5," ",E5," $TEMPO dport=",H5,"' |  $NC; sleep $((2*$TEMPO));")</f>
@@ -2476,7 +2468,7 @@
       </c>
       <c r="P6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H6,"'}, ")</f>
-        <v>'tp_dst':'11095'}, </v>
+        <v>'tp_dst':'11095'},</v>
       </c>
       <c r="R6" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("echo '$USR|",C6," ",E6," $TEMPO dport=",H6,"' |  $NC; sleep $((2*$TEMPO));")</f>
@@ -2534,7 +2526,7 @@
       </c>
       <c r="P7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H7,"'}, ")</f>
-        <v>'tp_dst':'443'}, </v>
+        <v>'tp_dst':'443'},</v>
       </c>
       <c r="R7" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("echo '$USR|",C7," ",E7," $TEMPO dport=",H7,"' |  $NC; sleep $((2*$TEMPO));")</f>
@@ -2592,7 +2584,7 @@
       </c>
       <c r="P8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H8,"'}, ")</f>
-        <v>'tp_dst':'80'}, </v>
+        <v>'tp_dst':'80'},</v>
       </c>
       <c r="R8" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("echo '$USR|",C8," ",E8," $TEMPO dport=",H8,"' |  $NC; sleep $((2*$TEMPO));")</f>
@@ -2653,7 +2645,7 @@
       </c>
       <c r="P10" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H10,"'}, ")</f>
-        <v>'tp_dst':'23'}, </v>
+        <v>'tp_dst':'23'},</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2707,7 +2699,7 @@
       </c>
       <c r="P11" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H11,"'}, ")</f>
-        <v>'tp_dst':'2323'}, </v>
+        <v>'tp_dst':'2323'},</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2761,7 +2753,7 @@
       </c>
       <c r="P12" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H12,"'}, ")</f>
-        <v>'tp_dst':'48101'}, </v>
+        <v>'tp_dst':'48101'},</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2815,7 +2807,7 @@
       </c>
       <c r="P13" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H13,"'}, ")</f>
-        <v>'tp_dst':'any'}, </v>
+        <v>'tp_dst':'any'},</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2869,7 +2861,7 @@
       </c>
       <c r="P14" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H14,"'}, ")</f>
-        <v>'tp_dst':'any'}, </v>
+        <v>'tp_dst':'any'},</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2923,7 +2915,7 @@
       </c>
       <c r="P15" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H15,"'}, ")</f>
-        <v>'tp_dst':'any'}, </v>
+        <v>'tp_dst':'any'},</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2980,7 +2972,7 @@
       </c>
       <c r="P17" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H17,"'}, ")</f>
-        <v>'tp_dst':'any'}, </v>
+        <v>'tp_dst':'any'},</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3034,7 +3026,7 @@
       </c>
       <c r="P18" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H18,"'}, ")</f>
-        <v>'tp_dst':'any'}, </v>
+        <v>'tp_dst':'any'},</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3088,7 +3080,7 @@
       </c>
       <c r="P19" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H19,"'}, ")</f>
-        <v>'tp_dst':'23'}, </v>
+        <v>'tp_dst':'23'},</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3142,7 +3134,7 @@
       </c>
       <c r="P20" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H20,"'}, ")</f>
-        <v>'tp_dst':'2323'}, </v>
+        <v>'tp_dst':'2323'},</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3253,12 +3245,118 @@
       </c>
       <c r="P23" s="1" t="str">
         <f aca="false">_xlfn.CONCAT("'tp_dst':'",H23,"'}, ")</f>
+        <v>'tp_dst':'any'},</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="J25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'type':'",A25,"',")</f>
+        <v>{'type':'M_N_ATK',</v>
+      </c>
+      <c r="K25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'name':'",B25,"-",C25,"',")</f>
+        <v>'name':'mirai_infect_v4from-bin_download_from',</v>
+      </c>
+      <c r="L25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",D25,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="M25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",E25,"',")</f>
+        <v>'nw_dst':'192.168.5.1',</v>
+      </c>
+      <c r="N25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",F25,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="O25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",G25,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="P25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",H25,"'}, ")</f>
+        <v>'tp_dst':'80'}, </v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'type':'",A26,"',")</f>
+        <v>{'type':'M_N_ATK',</v>
+      </c>
+      <c r="K26" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'name':'",B26,"-",C26,"',")</f>
+        <v>'name':'mirai_infect_v4to-bin_download_to',</v>
+      </c>
+      <c r="L26" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",D26,"',")</f>
+        <v>'nw_src':'192.168.5.1',</v>
+      </c>
+      <c r="M26" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",E26,"',")</f>
+        <v>'nw_dst':'thing',</v>
+      </c>
+      <c r="N26" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",F26,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="O26" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",G26,"',")</f>
+        <v>'tp_src':'80',</v>
+      </c>
+      <c r="P26" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",H26,"'}, ")</f>
         <v>'tp_dst':'any'}, </v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
add mtd2 file for experiment
</commit_message>
<xml_diff>
--- a/experiment/data/mirai_mtd.xlsx
+++ b/experiment/data/mirai_mtd.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Mirai" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="exp_base" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="exp_base_2" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="72">
   <si>
     <t xml:space="preserve">Group</t>
   </si>
@@ -229,6 +230,15 @@
   <si>
     <t xml:space="preserve">bin_download_to</t>
   </si>
+  <si>
+    <t xml:space="preserve">ALERT_T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RISK_T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RISK</t>
+  </si>
 </sst>
 </file>
 
@@ -338,18 +348,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -391,13 +401,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y1013"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.57"/>
@@ -408,8 +418,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="41.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.37"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="12" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="12" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2145,13 +2155,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF1006"/>
+  <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AA2" activeCellId="0" sqref="AA2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.88"/>
@@ -2169,7 +2179,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="16.6"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="17" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4419,4 +4429,2745 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AL26"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="32.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="32.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="33.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="33.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="1" width="23.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="26.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="16.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="X1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AG1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>443</v>
+      </c>
+      <c r="M2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A2,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B2,"',")</f>
+        <v>'acl-name':'mirai_ddos_v4from',</v>
+      </c>
+      <c r="O2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C2,",'risk':",D2,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':1},</v>
+      </c>
+      <c r="P2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E2,"',")</f>
+        <v>'ace-name':'udp',</v>
+      </c>
+      <c r="Q2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F2,",")</f>
+        <v>'ace-risk':1,</v>
+      </c>
+      <c r="R2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G2,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H2,"',")</f>
+        <v>'nw_dst':'172.217.29.110',</v>
+      </c>
+      <c r="T2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I2,"',")</f>
+        <v>'transport':'UDP',</v>
+      </c>
+      <c r="U2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J2,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K2,"'}, ")</f>
+        <v>'tp_dst':'443'}, </v>
+      </c>
+      <c r="X2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("echo '$USR|",E2," ",H2," $TEMPO dport=",K2,"' |  $NC; sleep $((2*$TEMPO));")</f>
+        <v>echo '$USR|udp 172.217.29.110 $TEMPO dport=443' |  $NC; sleep $((2*$TEMPO));</v>
+      </c>
+      <c r="AG2" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("priority=50,",LOWER(I2),",nw_dst=",H2,",tp_dst=",K2,",action=drop")</f>
+        <v>priority=50,udp,nw_dst=172.217.29.110,tp_dst=443,action=drop</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>27015</v>
+      </c>
+      <c r="M3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A3,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B3,"',")</f>
+        <v>'acl-name':'mirai_ddos_v4from',</v>
+      </c>
+      <c r="O3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C3,",'risk':",D3,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':1},</v>
+      </c>
+      <c r="P3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E3,"',")</f>
+        <v>'ace-name':'vse',</v>
+      </c>
+      <c r="Q3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F3,",")</f>
+        <v>'ace-risk':1,</v>
+      </c>
+      <c r="R3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G3,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H3,"',")</f>
+        <v>'nw_dst':'52.94.209.132',</v>
+      </c>
+      <c r="T3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I3,"',")</f>
+        <v>'transport':'UDP',</v>
+      </c>
+      <c r="U3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J3,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K3,"'}, ")</f>
+        <v>'tp_dst':'27015'}, </v>
+      </c>
+      <c r="X3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("echo '$USR|",E3," ",H3," $TEMPO dport=",K3,"' |  $NC; sleep $((2*$TEMPO));")</f>
+        <v>echo '$USR|vse 52.94.209.132 $TEMPO dport=27015' |  $NC; sleep $((2*$TEMPO));</v>
+      </c>
+      <c r="AG3" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("priority=50,",LOWER(I3),",nw_dst=",H3,",tp_dst=",K3,",action=drop")</f>
+        <v>priority=50,udp,nw_dst=52.94.209.132,tp_dst=27015,action=drop</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A4,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B4,"',")</f>
+        <v>'acl-name':'mirai_ddos_v4from',</v>
+      </c>
+      <c r="O4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C4,",'risk':",D4,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':1},</v>
+      </c>
+      <c r="P4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E4,"',")</f>
+        <v>'ace-name':'udpplain',</v>
+      </c>
+      <c r="Q4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F4,",")</f>
+        <v>'ace-risk':1,</v>
+      </c>
+      <c r="R4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G4,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H4,"',")</f>
+        <v>'nw_dst':'130.149.17.8',</v>
+      </c>
+      <c r="T4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I4,"',")</f>
+        <v>'transport':'UDP',</v>
+      </c>
+      <c r="U4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J4,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K4,"'}, ")</f>
+        <v>'tp_dst':'123'}, </v>
+      </c>
+      <c r="X4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("echo '$USR|",E4," ",H4," $TEMPO dport=",K4,"' |  $NC; sleep $((2*$TEMPO));")</f>
+        <v>echo '$USR|udpplain 130.149.17.8 $TEMPO dport=123' |  $NC; sleep $((2*$TEMPO));</v>
+      </c>
+      <c r="AG4" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("priority=50,",LOWER(I4),",nw_dst=",H4,",tp_dst=",K4,",action=drop")</f>
+        <v>priority=50,udp,nw_dst=130.149.17.8,tp_dst=123,action=drop</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="M5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A5,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B5,"',")</f>
+        <v>'acl-name':'mirai_ddos_v4from',</v>
+      </c>
+      <c r="O5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C5,",'risk':",D5,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':1},</v>
+      </c>
+      <c r="P5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E5,"',")</f>
+        <v>'ace-name':'syn',</v>
+      </c>
+      <c r="Q5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F5,",")</f>
+        <v>'ace-risk':1,</v>
+      </c>
+      <c r="R5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G5,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H5,"',")</f>
+        <v>'nw_dst':'93.184.216.34',</v>
+      </c>
+      <c r="T5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I5,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J5,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K5,"'}, ")</f>
+        <v>'tp_dst':'80'}, </v>
+      </c>
+      <c r="X5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("echo '$USR|",E5," ",H5," $TEMPO dport=",K5,"' |  $NC; sleep $((2*$TEMPO));")</f>
+        <v>echo '$USR|syn 93.184.216.34 $TEMPO dport=80' |  $NC; sleep $((2*$TEMPO));</v>
+      </c>
+      <c r="AG5" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("priority=50,",LOWER(I5),",nw_dst=",H5,",tp_dst=",K5,",action=drop")</f>
+        <v>priority=50,tcp,nw_dst=93.184.216.34,tp_dst=80,action=drop</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>11095</v>
+      </c>
+      <c r="M6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A6,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B6,"',")</f>
+        <v>'acl-name':'mirai_ddos_v4from',</v>
+      </c>
+      <c r="O6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C6,",'risk':",D6,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':1},</v>
+      </c>
+      <c r="P6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E6,"',")</f>
+        <v>'ace-name':'ack',</v>
+      </c>
+      <c r="Q6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F6,",")</f>
+        <v>'ace-risk':1,</v>
+      </c>
+      <c r="R6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G6,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H6,"',")</f>
+        <v>'nw_dst':'35.174.82.237',</v>
+      </c>
+      <c r="T6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I6,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J6,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K6,"'}, ")</f>
+        <v>'tp_dst':'11095'}, </v>
+      </c>
+      <c r="X6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("echo '$USR|",E6," ",H6," $TEMPO dport=",K6,"' |  $NC; sleep $((2*$TEMPO));")</f>
+        <v>echo '$USR|ack 35.174.82.237 $TEMPO dport=11095' |  $NC; sleep $((2*$TEMPO));</v>
+      </c>
+      <c r="AG6" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("priority=50,",LOWER(I6),",nw_dst=",H6,",tp_dst=",K6,",action=drop")</f>
+        <v>priority=50,tcp,nw_dst=35.174.82.237,tp_dst=11095,action=drop</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>443</v>
+      </c>
+      <c r="M7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A7,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B7,"',")</f>
+        <v>'acl-name':'mirai_ddos_v4from',</v>
+      </c>
+      <c r="O7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C7,",'risk':",D7,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':1},</v>
+      </c>
+      <c r="P7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E7,"',")</f>
+        <v>'ace-name':'stomp',</v>
+      </c>
+      <c r="Q7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F7,",")</f>
+        <v>'ace-risk':1,</v>
+      </c>
+      <c r="R7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G7,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H7,"',")</f>
+        <v>'nw_dst':'34.240.169.254',</v>
+      </c>
+      <c r="T7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I7,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J7,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K7,"'}, ")</f>
+        <v>'tp_dst':'443'}, </v>
+      </c>
+      <c r="X7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("echo '$USR|",E7," ",H7," $TEMPO dport=",K7,"' |  $NC; sleep $((2*$TEMPO));")</f>
+        <v>echo '$USR|stomp 34.240.169.254 $TEMPO dport=443' |  $NC; sleep $((2*$TEMPO));</v>
+      </c>
+      <c r="AG7" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("priority=50,",LOWER(I7),",nw_dst=",H7,",tp_dst=",K7,",action=drop")</f>
+        <v>priority=50,tcp,nw_dst=34.240.169.254,tp_dst=443,action=drop</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="M8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A8,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B8,"',")</f>
+        <v>'acl-name':'mirai_ddos_v4from',</v>
+      </c>
+      <c r="O8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C8,",'risk':",D8,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':1},</v>
+      </c>
+      <c r="P8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E8,"',")</f>
+        <v>'ace-name':'http',</v>
+      </c>
+      <c r="Q8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F8,",")</f>
+        <v>'ace-risk':1,</v>
+      </c>
+      <c r="R8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G8,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H8,"',")</f>
+        <v>'nw_dst':'176.32.98.203',</v>
+      </c>
+      <c r="T8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I8,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J8,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K8,"'}, ")</f>
+        <v>'tp_dst':'80'}, </v>
+      </c>
+      <c r="X8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("echo '$USR|",E8," ",H8," $TEMPO dport=",K8,"' |  $NC; sleep $((2*$TEMPO));")</f>
+        <v>echo '$USR|http 176.32.98.203 $TEMPO dport=80' |  $NC; sleep $((2*$TEMPO));</v>
+      </c>
+      <c r="AG8" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("priority=50,",LOWER(I8),",nw_dst=",H8,",tp_dst=",K8,",action=drop")</f>
+        <v>priority=50,tcp,nw_dst=176.32.98.203,tp_dst=80,action=drop</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="M10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A10,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B10,"',")</f>
+        <v>'acl-name':'mirai_scan_v4from',</v>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C10,",'risk':",D10,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':11},</v>
+      </c>
+      <c r="P10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E10,"',")</f>
+        <v>'ace-name':'scan_23_from',</v>
+      </c>
+      <c r="Q10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F10,",")</f>
+        <v>'ace-risk':10,</v>
+      </c>
+      <c r="R10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G10,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H10,"',")</f>
+        <v>'nw_dst':'local',</v>
+      </c>
+      <c r="T10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I10,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J10,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V10" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K10,"'}, ")</f>
+        <v>'tp_dst':'23'}, </v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>2323</v>
+      </c>
+      <c r="M11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A11,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B11,"',")</f>
+        <v>'acl-name':'mirai_scan_v4from',</v>
+      </c>
+      <c r="O11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C11,",'risk':",D11,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':11},</v>
+      </c>
+      <c r="P11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E11,"',")</f>
+        <v>'ace-name':'scan_2323_from',</v>
+      </c>
+      <c r="Q11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F11,",")</f>
+        <v>'ace-risk':10,</v>
+      </c>
+      <c r="R11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G11,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H11,"',")</f>
+        <v>'nw_dst':'local',</v>
+      </c>
+      <c r="T11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I11,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J11,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V11" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K11,"'}, ")</f>
+        <v>'tp_dst':'2323'}, </v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>48101</v>
+      </c>
+      <c r="M12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A12,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B12,"',")</f>
+        <v>'acl-name':'mirai_scan_v4from',</v>
+      </c>
+      <c r="O12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C12,",'risk':",D12,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':11},</v>
+      </c>
+      <c r="P12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E12,"',")</f>
+        <v>'ace-name':'scan_report_from',</v>
+      </c>
+      <c r="Q12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F12,",")</f>
+        <v>'ace-risk':1,</v>
+      </c>
+      <c r="R12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G12,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H12,"',")</f>
+        <v>'nw_dst':'192.168.5.1',</v>
+      </c>
+      <c r="T12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I12,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J12,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V12" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K12,"'}, ")</f>
+        <v>'tp_dst':'48101'}, </v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A13,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B13,"',")</f>
+        <v>'acl-name':'mirai_scan_v4to',</v>
+      </c>
+      <c r="O13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C13,",'risk':",D13,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':11},</v>
+      </c>
+      <c r="P13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E13,"',")</f>
+        <v>'ace-name':'scan_23_to',</v>
+      </c>
+      <c r="Q13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F13,",")</f>
+        <v>'ace-risk':10,</v>
+      </c>
+      <c r="R13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G13,"',")</f>
+        <v>'nw_src':'local',</v>
+      </c>
+      <c r="S13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H13,"',")</f>
+        <v>'nw_dst':'thing',</v>
+      </c>
+      <c r="T13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I13,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J13,"',")</f>
+        <v>'tp_src':'23',</v>
+      </c>
+      <c r="V13" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K13,"'}, ")</f>
+        <v>'tp_dst':'any'}, </v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>2323</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A14,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B14,"',")</f>
+        <v>'acl-name':'mirai_scan_v4to',</v>
+      </c>
+      <c r="O14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C14,",'risk':",D14,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':11},</v>
+      </c>
+      <c r="P14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E14,"',")</f>
+        <v>'ace-name':'scan_2323_to',</v>
+      </c>
+      <c r="Q14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F14,",")</f>
+        <v>'ace-risk':10,</v>
+      </c>
+      <c r="R14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G14,"',")</f>
+        <v>'nw_src':'local',</v>
+      </c>
+      <c r="S14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H14,"',")</f>
+        <v>'nw_dst':'thing',</v>
+      </c>
+      <c r="T14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I14,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J14,"',")</f>
+        <v>'tp_src':'2323',</v>
+      </c>
+      <c r="V14" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K14,"'}, ")</f>
+        <v>'tp_dst':'any'}, </v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <v>48101</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A15,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B15,"',")</f>
+        <v>'acl-name':'mirai_scan_v4to',</v>
+      </c>
+      <c r="O15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C15,",'risk':",D15,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':11},</v>
+      </c>
+      <c r="P15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E15,"',")</f>
+        <v>'ace-name':'scan_report_to',</v>
+      </c>
+      <c r="Q15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F15,",")</f>
+        <v>'ace-risk':1,</v>
+      </c>
+      <c r="R15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G15,"',")</f>
+        <v>'nw_src':'192.168.5.1',</v>
+      </c>
+      <c r="S15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H15,"',")</f>
+        <v>'nw_dst':'thing',</v>
+      </c>
+      <c r="T15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I15,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J15,"',")</f>
+        <v>'tp_src':'48101',</v>
+      </c>
+      <c r="V15" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K15,"'}, ")</f>
+        <v>'tp_dst':'any'}, </v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A17,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B17,"',")</f>
+        <v>'acl-name':'mirai_infect_v4from',</v>
+      </c>
+      <c r="O17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C17,",'risk':",D17,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':11},</v>
+      </c>
+      <c r="P17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E17,"',")</f>
+        <v>'ace-name':'infect_23_from',</v>
+      </c>
+      <c r="Q17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F17,",")</f>
+        <v>'ace-risk':10,</v>
+      </c>
+      <c r="R17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G17,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H17,"',")</f>
+        <v>'nw_dst':'192.168.5.1',</v>
+      </c>
+      <c r="T17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I17,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J17,"',")</f>
+        <v>'tp_src':'23',</v>
+      </c>
+      <c r="V17" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K17,"'}, ")</f>
+        <v>'tp_dst':'any'}, </v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="1" t="n">
+        <v>2323</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A18,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B18,"',")</f>
+        <v>'acl-name':'mirai_infect_v4from',</v>
+      </c>
+      <c r="O18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C18,",'risk':",D18,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':11},</v>
+      </c>
+      <c r="P18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E18,"',")</f>
+        <v>'ace-name':'infect_2323_from',</v>
+      </c>
+      <c r="Q18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F18,",")</f>
+        <v>'ace-risk':10,</v>
+      </c>
+      <c r="R18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G18,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H18,"',")</f>
+        <v>'nw_dst':'192.168.5.1',</v>
+      </c>
+      <c r="T18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I18,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J18,"',")</f>
+        <v>'tp_src':'2323',</v>
+      </c>
+      <c r="V18" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K18,"'}, ")</f>
+        <v>'tp_dst':'any'}, </v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="M19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A19,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B19,"',")</f>
+        <v>'acl-name':'mirai_infect_v4to',</v>
+      </c>
+      <c r="O19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C19,",'risk':",D19,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':11},</v>
+      </c>
+      <c r="P19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E19,"',")</f>
+        <v>'ace-name':'infect_23_to',</v>
+      </c>
+      <c r="Q19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F19,",")</f>
+        <v>'ace-risk':10,</v>
+      </c>
+      <c r="R19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G19,"',")</f>
+        <v>'nw_src':'192.168.5.1',</v>
+      </c>
+      <c r="S19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H19,"',")</f>
+        <v>'nw_dst':'thing',</v>
+      </c>
+      <c r="T19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I19,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J19,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V19" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K19,"'}, ")</f>
+        <v>'tp_dst':'23'}, </v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="1" t="n">
+        <v>2323</v>
+      </c>
+      <c r="M20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A20,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B20,"',")</f>
+        <v>'acl-name':'mirai_infect_v4to',</v>
+      </c>
+      <c r="O20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C20,",'risk':",D20,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':11},</v>
+      </c>
+      <c r="P20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E20,"',")</f>
+        <v>'ace-name':'infect_2323_to',</v>
+      </c>
+      <c r="Q20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F20,",")</f>
+        <v>'ace-risk':10,</v>
+      </c>
+      <c r="R20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G20,"',")</f>
+        <v>'nw_src':'192.168.5.1',</v>
+      </c>
+      <c r="S20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H20,"',")</f>
+        <v>'nw_dst':'thing',</v>
+      </c>
+      <c r="T20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I20,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J20,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V20" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K20,"'}, ")</f>
+        <v>'tp_dst':'2323'}, </v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="M21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A21,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B21,"',")</f>
+        <v>'acl-name':'mirai_infect_v4from',</v>
+      </c>
+      <c r="O21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C21,",'risk':",D21,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':11},</v>
+      </c>
+      <c r="P21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E21,"',")</f>
+        <v>'ace-name':'bin_download_from',</v>
+      </c>
+      <c r="Q21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F21,",")</f>
+        <v>'ace-risk':1,</v>
+      </c>
+      <c r="R21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G21,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H21,"',")</f>
+        <v>'nw_dst':'192.168.5.1',</v>
+      </c>
+      <c r="T21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I21,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J21,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V21" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K21,"'}, ")</f>
+        <v>'tp_dst':'80'}, </v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M22" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A22,"',")</f>
+        <v>{'group':'M_ATK',</v>
+      </c>
+      <c r="N22" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B22,"',")</f>
+        <v>'acl-name':'mirai_infect_v4to',</v>
+      </c>
+      <c r="O22" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C22,",'risk':",D22,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':11},</v>
+      </c>
+      <c r="P22" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E22,"',")</f>
+        <v>'ace-name':'bin_download_to',</v>
+      </c>
+      <c r="Q22" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F22,",")</f>
+        <v>'ace-risk':1,</v>
+      </c>
+      <c r="R22" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G22,"',")</f>
+        <v>'nw_src':'192.168.5.1',</v>
+      </c>
+      <c r="S22" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H22,"',")</f>
+        <v>'nw_dst':'thing',</v>
+      </c>
+      <c r="T22" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I22,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U22" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J22,"',")</f>
+        <v>'tp_src':'80',</v>
+      </c>
+      <c r="V22" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K22,"'}, ")</f>
+        <v>'tp_dst':'any'}, </v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>2030</v>
+      </c>
+      <c r="M24" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A24,"',")</f>
+        <v>{'group':'M_N_ATK',</v>
+      </c>
+      <c r="N24" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B24,"',")</f>
+        <v>'acl-name':'mirai_cnc_v4from',</v>
+      </c>
+      <c r="O24" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C24,",'risk':",D24,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':1},</v>
+      </c>
+      <c r="P24" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E24,"',")</f>
+        <v>'ace-name':'cnc_socket_from',</v>
+      </c>
+      <c r="Q24" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F24,",")</f>
+        <v>'ace-risk':1,</v>
+      </c>
+      <c r="R24" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G24,"',")</f>
+        <v>'nw_src':'thing',</v>
+      </c>
+      <c r="S24" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H24,"',")</f>
+        <v>'nw_dst':'192.168.5.1',</v>
+      </c>
+      <c r="T24" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I24,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U24" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J24,"',")</f>
+        <v>'tp_src':'any',</v>
+      </c>
+      <c r="V24" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K24,"'}, ")</f>
+        <v>'tp_dst':'2030'}, </v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="1" t="n">
+        <v>2030</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("{'group':'",A25,"',")</f>
+        <v>{'group':'M_N_ATK',</v>
+      </c>
+      <c r="N25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-name':'",B25,"',")</f>
+        <v>'acl-name':'mirai_cnc_v4to',</v>
+      </c>
+      <c r="O25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'acl-thresholds':{'alert':",C25,",'risk':",D25,"},")</f>
+        <v>'acl-thresholds':{'alert':1,'risk':1},</v>
+      </c>
+      <c r="P25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-name':'",E25,"',")</f>
+        <v>'ace-name':'cnc_socket_to',</v>
+      </c>
+      <c r="Q25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'ace-risk':",F25,",")</f>
+        <v>'ace-risk':1,</v>
+      </c>
+      <c r="R25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_src':'",G25,"',")</f>
+        <v>'nw_src':'192.168.5.1',</v>
+      </c>
+      <c r="S25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'nw_dst':'",H25,"',")</f>
+        <v>'nw_dst':'thing',</v>
+      </c>
+      <c r="T25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'transport':'",I25,"',")</f>
+        <v>'transport':'TCP',</v>
+      </c>
+      <c r="U25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_src':'",J25,"',")</f>
+        <v>'tp_src':'2030',</v>
+      </c>
+      <c r="V25" s="1" t="str">
+        <f aca="false">_xlfn.CONCAT("'tp_dst':'",K25,"'}, ")</f>
+        <v>'tp_dst':'any'}, </v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1006" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1007" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1008" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="M1:V1"/>
+    <mergeCell ref="X1:AE1"/>
+    <mergeCell ref="AG1:AL1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>